<commit_message>
Restored functionality of unique_molecule counting function
</commit_message>
<xml_diff>
--- a/test_short/heatmaps/new_count.xlsx
+++ b/test_short/heatmaps/new_count.xlsx
@@ -498,34 +498,34 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>2892</v>
+        <v>2882</v>
       </c>
       <c r="D2" t="n">
-        <v>2860</v>
+        <v>2842</v>
       </c>
       <c r="E2" t="n">
-        <v>1495</v>
+        <v>1487</v>
       </c>
       <c r="F2" t="n">
-        <v>2887</v>
+        <v>2882</v>
       </c>
       <c r="G2" t="n">
-        <v>1479</v>
+        <v>2431</v>
       </c>
       <c r="H2" t="n">
-        <v>1458</v>
+        <v>2251</v>
       </c>
       <c r="I2" t="n">
-        <v>1465</v>
+        <v>2250</v>
       </c>
       <c r="J2" t="n">
-        <v>1459</v>
+        <v>2251</v>
       </c>
       <c r="K2" t="n">
-        <v>1474</v>
+        <v>2430</v>
       </c>
       <c r="L2" t="n">
-        <v>2887</v>
+        <v>2882</v>
       </c>
     </row>
     <row r="3">
@@ -548,19 +548,19 @@
         <v>121</v>
       </c>
       <c r="G3" t="n">
-        <v>86</v>
+        <v>190</v>
       </c>
       <c r="H3" t="n">
-        <v>154</v>
+        <v>190</v>
       </c>
       <c r="I3" t="n">
-        <v>88</v>
+        <v>190</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="L3" t="n">
         <v>121</v>
@@ -576,32 +576,32 @@
         <v>748</v>
       </c>
       <c r="C4" t="n">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F4" t="n">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="G4" t="n">
-        <v>364</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>282</v>
+        <v>628</v>
       </c>
       <c r="I4" t="n">
-        <v>282</v>
+        <v>628</v>
       </c>
       <c r="J4" t="n">
-        <v>281</v>
+        <v>628</v>
       </c>
       <c r="K4" t="n">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="5">
@@ -624,22 +624,22 @@
         <v>288</v>
       </c>
       <c r="G5" t="n">
-        <v>306</v>
+        <v>465</v>
       </c>
       <c r="H5" t="n">
-        <v>306</v>
+        <v>465</v>
       </c>
       <c r="I5" t="n">
-        <v>306</v>
+        <v>465</v>
       </c>
       <c r="J5" t="n">
-        <v>306</v>
+        <v>465</v>
       </c>
       <c r="K5" t="n">
-        <v>306</v>
+        <v>465</v>
       </c>
       <c r="L5" t="n">
-        <v>288</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6">
@@ -649,35 +649,35 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>684</v>
+        <v>1038</v>
       </c>
       <c r="C6" t="n">
-        <v>342</v>
+        <v>520</v>
       </c>
       <c r="D6" t="n">
-        <v>684</v>
+        <v>1038</v>
       </c>
       <c r="E6" t="n">
-        <v>342</v>
+        <v>520</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
-        <v>288</v>
+        <v>767</v>
       </c>
       <c r="H6" t="n">
-        <v>332</v>
+        <v>800</v>
       </c>
       <c r="I6" t="n">
-        <v>352</v>
+        <v>751</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>751</v>
       </c>
       <c r="K6" t="n">
-        <v>122</v>
+        <v>721</v>
       </c>
       <c r="L6" t="n">
-        <v>342</v>
+        <v>520</v>
       </c>
     </row>
     <row r="7">
@@ -687,35 +687,35 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>488</v>
+        <v>1365</v>
       </c>
       <c r="C7" t="n">
-        <v>488</v>
+        <v>1363</v>
       </c>
       <c r="D7" t="n">
-        <v>488</v>
+        <v>1365</v>
       </c>
       <c r="E7" t="n">
-        <v>488</v>
+        <v>1360</v>
       </c>
       <c r="F7" t="n">
-        <v>488</v>
+        <v>1452</v>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>176</v>
+        <v>1452</v>
       </c>
       <c r="I7" t="n">
-        <v>312</v>
+        <v>1365</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>1365</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>1365</v>
       </c>
       <c r="L7" t="n">
-        <v>488</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="8">
@@ -725,35 +725,35 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>252</v>
+        <v>511</v>
       </c>
       <c r="C8" t="n">
-        <v>252</v>
+        <v>511</v>
       </c>
       <c r="D8" t="n">
-        <v>252</v>
+        <v>511</v>
       </c>
       <c r="E8" t="n">
-        <v>252</v>
+        <v>510</v>
       </c>
       <c r="F8" t="n">
-        <v>252</v>
+        <v>554</v>
       </c>
       <c r="G8" t="n">
-        <v>139</v>
+        <v>554</v>
       </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>511</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>511</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>511</v>
       </c>
       <c r="L8" t="n">
-        <v>252</v>
+        <v>510</v>
       </c>
     </row>
     <row r="9">
@@ -778,7 +778,7 @@
         <v>408</v>
       </c>
       <c r="G9" t="n">
-        <v>90</v>
+        <v>408</v>
       </c>
       <c r="H9" t="n">
         <v>408</v>
@@ -788,7 +788,7 @@
         <v>408</v>
       </c>
       <c r="K9" t="n">
-        <v>90</v>
+        <v>408</v>
       </c>
       <c r="L9" t="n">
         <v>408</v>
@@ -816,7 +816,7 @@
         <v>310</v>
       </c>
       <c r="G10" t="n">
-        <v>139</v>
+        <v>310</v>
       </c>
       <c r="H10" t="n">
         <v>310</v>
@@ -857,10 +857,10 @@
         <v>443</v>
       </c>
       <c r="H11" t="n">
-        <v>132</v>
+        <v>443</v>
       </c>
       <c r="I11" t="n">
-        <v>132</v>
+        <v>443</v>
       </c>
       <c r="J11" t="n">
         <v>443</v>
@@ -892,19 +892,19 @@
         <v>531</v>
       </c>
       <c r="G12" t="n">
-        <v>431</v>
+        <v>767</v>
       </c>
       <c r="H12" t="n">
-        <v>661</v>
+        <v>861</v>
       </c>
       <c r="I12" t="n">
-        <v>661</v>
+        <v>861</v>
       </c>
       <c r="J12" t="n">
-        <v>661</v>
+        <v>861</v>
       </c>
       <c r="K12" t="n">
-        <v>170</v>
+        <v>767</v>
       </c>
       <c r="L12" t="inlineStr"/>
     </row>

</xml_diff>